<commit_message>
Start the firm Morgan.
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Sheet.xlsx
+++ b/src/baseFiles/excel/Sheet.xlsx
@@ -436,16 +436,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v/>
+        <v>Mark</v>
       </c>
       <c r="B2" t="str">
-        <v/>
+        <v>Mark Dillon</v>
       </c>
       <c r="C2" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D2" t="str">
-        <v/>
+        <v>Ireland</v>
       </c>
       <c r="E2" t="str">
         <v/>
@@ -454,7 +454,7 @@
         <v/>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>mark.dillon@dechert.com</v>
       </c>
       <c r="P2" t="str">
         <v>Afghanistan</v>
@@ -564,16 +564,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v/>
+        <v>Jay</v>
       </c>
       <c r="B6" t="str">
-        <v/>
+        <v>Jay Jurata</v>
       </c>
       <c r="C6" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D6" t="str">
-        <v/>
+        <v>Not Found</v>
       </c>
       <c r="E6" t="str">
         <v/>
@@ -582,7 +582,7 @@
         <v/>
       </c>
       <c r="G6" t="str">
-        <v/>
+        <v>jay.jurata@dechert.com</v>
       </c>
       <c r="P6" t="str">
         <v>Anguilla</v>
@@ -756,16 +756,16 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v/>
+        <v>Olaf</v>
       </c>
       <c r="B12" t="str">
-        <v/>
+        <v>Olaf Fasshauer</v>
       </c>
       <c r="C12" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D12" t="str">
-        <v/>
+        <v>Germany</v>
       </c>
       <c r="E12" t="str">
         <v/>
@@ -774,7 +774,7 @@
         <v/>
       </c>
       <c r="G12" t="str">
-        <v/>
+        <v>olaf.fasshauer@dechert.com</v>
       </c>
       <c r="P12" t="str">
         <v>Austria</v>
@@ -884,16 +884,16 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v/>
+        <v>Arne</v>
       </c>
       <c r="B16" t="str">
-        <v/>
+        <v>Arne Bolch</v>
       </c>
       <c r="C16" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D16" t="str">
-        <v/>
+        <v>Luxembourg</v>
       </c>
       <c r="E16" t="str">
         <v/>
@@ -902,7 +902,7 @@
         <v/>
       </c>
       <c r="G16" t="str">
-        <v/>
+        <v>arne.bolch@dechert.com</v>
       </c>
       <c r="P16" t="str">
         <v>Bangladesh</v>
@@ -916,16 +916,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v/>
+        <v>Eric</v>
       </c>
       <c r="B17" t="str">
-        <v/>
+        <v>G Eric Brunstad Jr</v>
       </c>
       <c r="C17" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D17" t="str">
-        <v/>
+        <v>Not Found</v>
       </c>
       <c r="E17" t="str">
         <v/>
@@ -934,7 +934,7 @@
         <v/>
       </c>
       <c r="G17" t="str">
-        <v/>
+        <v>eric.brunstad@dechert.com</v>
       </c>
       <c r="P17" t="str">
         <v>Barbados</v>
@@ -1012,16 +1012,16 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v/>
+        <v>Amanjit</v>
       </c>
       <c r="B20" t="str">
-        <v/>
+        <v>Amanjit K Fagura</v>
       </c>
       <c r="C20" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D20" t="str">
-        <v/>
+        <v>the UAE</v>
       </c>
       <c r="E20" t="str">
         <v/>
@@ -1030,7 +1030,7 @@
         <v/>
       </c>
       <c r="G20" t="str">
-        <v/>
+        <v>amanjit.fagura@dechert.com</v>
       </c>
       <c r="P20" t="str">
         <v>Belize</v>
@@ -1108,16 +1108,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v/>
+        <v>Dean</v>
       </c>
       <c r="B23" t="str">
-        <v/>
+        <v>Dean Collins</v>
       </c>
       <c r="C23" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D23" t="str">
-        <v/>
+        <v>Singapore</v>
       </c>
       <c r="E23" t="str">
         <v/>
@@ -1126,7 +1126,7 @@
         <v/>
       </c>
       <c r="G23" t="str">
-        <v/>
+        <v>dean.collins@dechert.com</v>
       </c>
       <c r="P23" t="str">
         <v>Bhutan</v>
@@ -1364,16 +1364,16 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v/>
+        <v>Eric</v>
       </c>
       <c r="B31" t="str">
-        <v/>
+        <v>Eric Deltour</v>
       </c>
       <c r="C31" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D31" t="str">
-        <v/>
+        <v>Belgium</v>
       </c>
       <c r="E31" t="str">
         <v/>
@@ -1382,7 +1382,7 @@
         <v/>
       </c>
       <c r="G31" t="str">
-        <v/>
+        <v>eric.deltour@dechert.com</v>
       </c>
       <c r="P31" t="str">
         <v>Bulgaria</v>
@@ -1556,16 +1556,16 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v/>
+        <v>Daniel</v>
       </c>
       <c r="B37" t="str">
-        <v/>
+        <v>Daniel Margulies</v>
       </c>
       <c r="C37" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D37" t="str">
-        <v/>
+        <v>Hong Kong</v>
       </c>
       <c r="E37" t="str">
         <v/>
@@ -1574,7 +1574,7 @@
         <v/>
       </c>
       <c r="G37" t="str">
-        <v/>
+        <v>daniel.margulies@dechert.com</v>
       </c>
       <c r="P37" t="str">
         <v>Cape Verde</v>
@@ -1652,16 +1652,16 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v/>
+        <v>Karen</v>
       </c>
       <c r="B40" t="str">
-        <v/>
+        <v>Karen L Anderberg</v>
       </c>
       <c r="C40" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D40" t="str">
-        <v/>
+        <v>England</v>
       </c>
       <c r="E40" t="str">
         <v/>
@@ -1670,7 +1670,7 @@
         <v/>
       </c>
       <c r="G40" t="str">
-        <v/>
+        <v>karen.anderberg@dechert.com</v>
       </c>
       <c r="P40" t="str">
         <v>Chad</v>
@@ -1812,16 +1812,16 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v/>
+        <v>Stephen</v>
       </c>
       <c r="B45" t="str">
-        <v/>
+        <v>Stephen D Zide</v>
       </c>
       <c r="C45" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D45" t="str">
-        <v/>
+        <v>Not Found</v>
       </c>
       <c r="E45" t="str">
         <v/>
@@ -1830,7 +1830,7 @@
         <v/>
       </c>
       <c r="G45" t="str">
-        <v/>
+        <v>stephen.zide@dechert.com</v>
       </c>
       <c r="P45" t="str">
         <v>Cook Islands</v>
@@ -1972,16 +1972,16 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v/>
+        <v>Olivia</v>
       </c>
       <c r="B50" t="str">
-        <v/>
+        <v>Olivia Bernardeau-Paupe</v>
       </c>
       <c r="C50" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D50" t="str">
-        <v/>
+        <v>France</v>
       </c>
       <c r="E50" t="str">
         <v/>
@@ -1990,7 +1990,7 @@
         <v/>
       </c>
       <c r="G50" t="str">
-        <v/>
+        <v>olivia.bernardeaupaupe@dechert.com</v>
       </c>
       <c r="P50" t="str">
         <v>Cyprus</v>
@@ -2004,16 +2004,16 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v/>
+        <v>Amanda</v>
       </c>
       <c r="B51" t="str">
-        <v/>
+        <v>Amanda K Antons Ph D</v>
       </c>
       <c r="C51" t="str">
-        <v/>
+        <v>Dechert LLP</v>
       </c>
       <c r="D51" t="str">
-        <v/>
+        <v>Dominican Republic</v>
       </c>
       <c r="E51" t="str">
         <v/>
@@ -2022,7 +2022,7 @@
         <v/>
       </c>
       <c r="G51" t="str">
-        <v/>
+        <v>amanda.antons@dechert.com</v>
       </c>
       <c r="P51" t="str">
         <v>Czech Republic</v>

</xml_diff>

<commit_message>
Just before a test
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Sheet.xlsx
+++ b/src/baseFiles/excel/Sheet.xlsx
@@ -1428,16 +1428,16 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v/>
+        <v>Bingna</v>
       </c>
       <c r="B33" t="str">
-        <v/>
+        <v>Bingna Guo</v>
       </c>
       <c r="C33" t="str">
-        <v/>
+        <v>Morgan Lewis And Bockius LLP</v>
       </c>
       <c r="D33" t="str">
-        <v/>
+        <v>China</v>
       </c>
       <c r="E33" t="str">
         <v/>
@@ -1446,7 +1446,7 @@
         <v/>
       </c>
       <c r="G33" t="str">
-        <v/>
+        <v>bingna.guo@morganlewis.com</v>
       </c>
       <c r="P33" t="str">
         <v>Burundi</v>

</xml_diff>

<commit_message>
Trying to implement the yield on the Site searchForLawyers. Create a BaseSite with common operations and Att of sites
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Sheet.xlsx
+++ b/src/baseFiles/excel/Sheet.xlsx
@@ -532,16 +532,16 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v/>
+        <v>Suzanne</v>
       </c>
       <c r="B5" t="str">
-        <v/>
+        <v>Suzanne Brooker</v>
       </c>
       <c r="C5" t="str">
-        <v/>
+        <v>Spencer West</v>
       </c>
       <c r="D5" t="str">
-        <v/>
+        <v>England</v>
       </c>
       <c r="E5" t="str">
         <v/>
@@ -550,7 +550,7 @@
         <v/>
       </c>
       <c r="G5" t="str">
-        <v/>
+        <v>suzanne.brooker@spencer-west.com</v>
       </c>
       <c r="P5" t="str">
         <v>Andorra</v>
@@ -1588,16 +1588,16 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v/>
+        <v>Suzanne</v>
       </c>
       <c r="B38" t="str">
-        <v/>
+        <v>Suzanne Brooker</v>
       </c>
       <c r="C38" t="str">
-        <v/>
+        <v>Spencer West</v>
       </c>
       <c r="D38" t="str">
-        <v/>
+        <v>England</v>
       </c>
       <c r="E38" t="str">
         <v/>
@@ -1606,7 +1606,7 @@
         <v/>
       </c>
       <c r="G38" t="str">
-        <v/>
+        <v>suzanne.brooker@spencer-west.com</v>
       </c>
       <c r="P38" t="str">
         <v>Cayman Islands</v>

</xml_diff>

<commit_message>
New Page problem fixed, more firms. Start to change the structure of registration in the base classes, need to test then in the specializations
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Sheet.xlsx
+++ b/src/baseFiles/excel/Sheet.xlsx
@@ -472,16 +472,16 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>=PROPER(IFERROR(LEFT(B3,FIND(" ",B3)-1),B3))</v>
+        <v>Olivier</v>
       </c>
       <c r="B3" t="str">
-        <v/>
+        <v>Olivier Chambord</v>
       </c>
       <c r="C3" t="str">
-        <v/>
+        <v>Morgan Lewis And Bockius LLP</v>
       </c>
       <c r="D3" t="str">
-        <v/>
+        <v>France</v>
       </c>
       <c r="E3" t="str">
         <v>=IFERROR(VLOOKUP(D3,P2:Q260,2,FALSE),"Not Found")</v>
@@ -490,7 +490,7 @@
         <v/>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>olivier.chambord@morganlewis.com</v>
       </c>
       <c r="P3" t="str">
         <v>Albania</v>
@@ -536,16 +536,16 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>=PROPER(IFERROR(LEFT(B5,FIND(" ",B5)-1),B5))</v>
+        <v>James</v>
       </c>
       <c r="B5" t="str">
-        <v/>
+        <v>James P Bradley</v>
       </c>
       <c r="C5" t="str">
-        <v/>
+        <v>Morgan Lewis And Bockius LLP</v>
       </c>
       <c r="D5" t="str">
-        <v/>
+        <v>Singapore</v>
       </c>
       <c r="E5" t="str">
         <v>=IFERROR(VLOOKUP(D5,P2:Q260,2,FALSE),"Not Found")</v>
@@ -554,7 +554,7 @@
         <v/>
       </c>
       <c r="G5" t="str">
-        <v/>
+        <v>james.bradley@morganlewis.com</v>
       </c>
       <c r="P5" t="str">
         <v>Andorra</v>
@@ -568,16 +568,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>=PROPER(IFERROR(LEFT(B6,FIND(" ",B6)-1),B6))</v>
+        <v>Alexandra</v>
       </c>
       <c r="B6" t="str">
-        <v/>
+        <v>Alexandra Rodina</v>
       </c>
       <c r="C6" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D6" t="str">
-        <v/>
+        <v>England</v>
       </c>
       <c r="E6" t="str">
         <v>=IFERROR(VLOOKUP(D6,P2:Q260,2,FALSE),"Not Found")</v>
@@ -586,7 +586,7 @@
         <v/>
       </c>
       <c r="G6" t="str">
-        <v/>
+        <v>alexandra.rodina@kennedyslaw.com</v>
       </c>
       <c r="P6" t="str">
         <v>Anguilla</v>
@@ -696,16 +696,16 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>=PROPER(IFERROR(LEFT(B10,FIND(" ",B10)-1),B10))</v>
+        <v>Tomoko</v>
       </c>
       <c r="B10" t="str">
-        <v/>
+        <v>Tomoko Fuminaga</v>
       </c>
       <c r="C10" t="str">
-        <v/>
+        <v>Morgan Lewis And Bockius LLP</v>
       </c>
       <c r="D10" t="str">
-        <v/>
+        <v>Japan</v>
       </c>
       <c r="E10" t="str">
         <v>=IFERROR(VLOOKUP(D10,P2:Q260,2,FALSE),"Not Found")</v>
@@ -714,7 +714,7 @@
         <v/>
       </c>
       <c r="G10" t="str">
-        <v/>
+        <v>tomoko.fuminaga@morganlewis.com</v>
       </c>
       <c r="P10" t="str">
         <v>Aruba</v>
@@ -760,16 +760,16 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>=PROPER(IFERROR(LEFT(B12,FIND(" ",B12)-1),B12))</v>
+        <v>Amanda</v>
       </c>
       <c r="B12" t="str">
-        <v/>
+        <v>Amanda Beaumont</v>
       </c>
       <c r="C12" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D12" t="str">
-        <v/>
+        <v>England</v>
       </c>
       <c r="E12" t="str">
         <v>=IFERROR(VLOOKUP(D12,P2:Q260,2,FALSE),"Not Found")</v>
@@ -778,7 +778,7 @@
         <v/>
       </c>
       <c r="G12" t="str">
-        <v/>
+        <v>amanda.beaumont@kennedyslaw.com</v>
       </c>
       <c r="P12" t="str">
         <v>Austria</v>
@@ -792,16 +792,16 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>=PROPER(IFERROR(LEFT(B13,FIND(" ",B13)-1),B13))</v>
+        <v>Alberto</v>
       </c>
       <c r="B13" t="str">
-        <v/>
+        <v>Alberto Bunge</v>
       </c>
       <c r="C13" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D13" t="str">
-        <v/>
+        <v>Argentina</v>
       </c>
       <c r="E13" t="str">
         <v>=IFERROR(VLOOKUP(D13,P2:Q260,2,FALSE),"Not Found")</v>
@@ -810,7 +810,7 @@
         <v/>
       </c>
       <c r="G13" t="str">
-        <v/>
+        <v>alberto.bunge@kennedyslaw.com</v>
       </c>
       <c r="P13" t="str">
         <v>Azerbaijan</v>
@@ -856,16 +856,16 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>=PROPER(IFERROR(LEFT(B15,FIND(" ",B15)-1),B15))</v>
+        <v>Andrea</v>
       </c>
       <c r="B15" t="str">
-        <v/>
+        <v>Andrea Dougall</v>
       </c>
       <c r="C15" t="str">
-        <v/>
+        <v>Morgan Lewis And Bockius LLP</v>
       </c>
       <c r="D15" t="str">
-        <v/>
+        <v>the UAE</v>
       </c>
       <c r="E15" t="str">
         <v>=IFERROR(VLOOKUP(D15,P2:Q260,2,FALSE),"Not Found")</v>
@@ -874,7 +874,7 @@
         <v/>
       </c>
       <c r="G15" t="str">
-        <v/>
+        <v>andrea.dougall@morganlewis.com</v>
       </c>
       <c r="P15" t="str">
         <v>Bahrain</v>
@@ -888,16 +888,16 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>=PROPER(IFERROR(LEFT(B16,FIND(" ",B16)-1),B16))</v>
+        <v>Bingna</v>
       </c>
       <c r="B16" t="str">
-        <v/>
+        <v>Bingna Guo</v>
       </c>
       <c r="C16" t="str">
-        <v/>
+        <v>Morgan Lewis And Bockius LLP</v>
       </c>
       <c r="D16" t="str">
-        <v/>
+        <v>China</v>
       </c>
       <c r="E16" t="str">
         <v>=IFERROR(VLOOKUP(D16,P2:Q260,2,FALSE),"Not Found")</v>
@@ -906,7 +906,7 @@
         <v/>
       </c>
       <c r="G16" t="str">
-        <v/>
+        <v>bingna.guo@morganlewis.com</v>
       </c>
       <c r="P16" t="str">
         <v>Bangladesh</v>
@@ -920,16 +920,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>=PROPER(IFERROR(LEFT(B17,FIND(" ",B17)-1),B17))</v>
+        <v>Alfonso</v>
       </c>
       <c r="B17" t="str">
-        <v/>
+        <v>Alfonso De Ramos</v>
       </c>
       <c r="C17" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D17" t="str">
-        <v/>
+        <v>Spain</v>
       </c>
       <c r="E17" t="str">
         <v>=IFERROR(VLOOKUP(D17,P2:Q260,2,FALSE),"Not Found")</v>
@@ -938,7 +938,7 @@
         <v/>
       </c>
       <c r="G17" t="str">
-        <v/>
+        <v>alfonso.deramos@kennedyslaw.com</v>
       </c>
       <c r="P17" t="str">
         <v>Barbados</v>
@@ -1112,16 +1112,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>=PROPER(IFERROR(LEFT(B23,FIND(" ",B23)-1),B23))</v>
+        <v>Adam</v>
       </c>
       <c r="B23" t="str">
-        <v/>
+        <v>Adam Longney</v>
       </c>
       <c r="C23" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D23" t="str">
-        <v/>
+        <v>England</v>
       </c>
       <c r="E23" t="str">
         <v>=IFERROR(VLOOKUP(D23,P2:Q260,2,FALSE),"Not Found")</v>
@@ -1130,7 +1130,7 @@
         <v/>
       </c>
       <c r="G23" t="str">
-        <v/>
+        <v>adam.longney@kennedyslaw.com</v>
       </c>
       <c r="P23" t="str">
         <v>Bhutan</v>
@@ -1464,16 +1464,16 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>=PROPER(IFERROR(LEFT(B34,FIND(" ",B34)-1),B34))</v>
+        <v>Nick</v>
       </c>
       <c r="B34" t="str">
-        <v/>
+        <v>Nick Bolter</v>
       </c>
       <c r="C34" t="str">
-        <v/>
+        <v>Morgan Lewis And Bockius LLP</v>
       </c>
       <c r="D34" t="str">
-        <v/>
+        <v>Belgium</v>
       </c>
       <c r="E34" t="str">
         <v>=IFERROR(VLOOKUP(D34,P2:Q260,2,FALSE),"Not Found")</v>
@@ -1482,7 +1482,7 @@
         <v/>
       </c>
       <c r="G34" t="str">
-        <v/>
+        <v>nick.bolter@morganlewis.com</v>
       </c>
       <c r="P34" t="str">
         <v>Cambodia</v>
@@ -1528,16 +1528,16 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>=PROPER(IFERROR(LEFT(B36,FIND(" ",B36)-1),B36))</v>
+        <v>Alex</v>
       </c>
       <c r="B36" t="str">
-        <v/>
+        <v>Alex Nurse</v>
       </c>
       <c r="C36" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D36" t="str">
-        <v/>
+        <v>England</v>
       </c>
       <c r="E36" t="str">
         <v>=IFERROR(VLOOKUP(D36,P2:Q260,2,FALSE),"Not Found")</v>
@@ -1546,7 +1546,7 @@
         <v/>
       </c>
       <c r="G36" t="str">
-        <v/>
+        <v>alex.nurse@kennedyslaw.com</v>
       </c>
       <c r="P36" t="str">
         <v>Canada</v>
@@ -1560,16 +1560,16 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>=PROPER(IFERROR(LEFT(B37,FIND(" ",B37)-1),B37))</v>
+        <v>Andy</v>
       </c>
       <c r="B37" t="str">
-        <v/>
+        <v>Andy Purssell</v>
       </c>
       <c r="C37" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D37" t="str">
-        <v/>
+        <v>England</v>
       </c>
       <c r="E37" t="str">
         <v>=IFERROR(VLOOKUP(D37,P2:Q260,2,FALSE),"Not Found")</v>
@@ -1578,7 +1578,7 @@
         <v/>
       </c>
       <c r="G37" t="str">
-        <v/>
+        <v>andrew.purssell@kennedyslaw.com</v>
       </c>
       <c r="P37" t="str">
         <v>Cape Verde</v>
@@ -1721,16 +1721,16 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>=PROPER(IFERROR(LEFT(B42,FIND(" ",B42)-1),B42))</v>
+        <v>Alistair</v>
       </c>
       <c r="B42" t="str">
-        <v/>
+        <v>Alistair Darroch</v>
       </c>
       <c r="C42" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D42" t="str">
-        <v/>
+        <v>New Zealand</v>
       </c>
       <c r="E42" t="str">
         <v>=IFERROR(VLOOKUP(D42,P2:Q260,2,FALSE),"Not Found")</v>
@@ -1739,7 +1739,7 @@
         <v/>
       </c>
       <c r="G42" t="str">
-        <v/>
+        <v>alistair.darroch@kennedyslaw.com</v>
       </c>
       <c r="P42" t="str">
         <v>China</v>
@@ -1881,16 +1881,16 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>=PROPER(IFERROR(LEFT(B47,FIND(" ",B47)-1),B47))</v>
+        <v>Alberto</v>
       </c>
       <c r="B47" t="str">
-        <v/>
+        <v>Alberto Torres</v>
       </c>
       <c r="C47" t="str">
-        <v/>
+        <v>Kennedys</v>
       </c>
       <c r="D47" t="str">
-        <v/>
+        <v>Mexico</v>
       </c>
       <c r="E47" t="str">
         <v>=IFERROR(VLOOKUP(D47,P2:Q260,2,FALSE),"Not Found")</v>
@@ -1899,7 +1899,7 @@
         <v/>
       </c>
       <c r="G47" t="str">
-        <v/>
+        <v>alberto.torres@kennedyslaw.com</v>
       </c>
       <c r="P47" t="str">
         <v>Cote D'ivoire</v>
@@ -2041,16 +2041,16 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>=PROPER(IFERROR(LEFT(B52,FIND(" ",B52)-1),B52))</v>
+        <v>Alexandre</v>
       </c>
       <c r="B52" t="str">
-        <v/>
+        <v>Alexandre Bailly</v>
       </c>
       <c r="C52" t="str">
-        <v/>
+        <v>Morgan Lewis And Bockius LLP</v>
       </c>
       <c r="D52" t="str">
-        <v/>
+        <v>France</v>
       </c>
       <c r="E52" t="str">
         <v>=IFERROR(VLOOKUP(D52,P2:Q260,2,FALSE),"Not Found")</v>
@@ -2059,7 +2059,7 @@
         <v/>
       </c>
       <c r="G52" t="str">
-        <v/>
+        <v>alexandre.bailly@morganlewis.com</v>
       </c>
       <c r="P52" t="str">
         <v>Democratic Republic of the Congo</v>

</xml_diff>

<commit_message>
Change the data to collect and the Sheet. Need to test
</commit_message>
<xml_diff>
--- a/src/baseFiles/excel/Sheet.xlsx
+++ b/src/baseFiles/excel/Sheet.xlsx
@@ -429,289 +429,24 @@
         <v>Country</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>https://www.giambronelaw.com/site/people/profile/olu.ajasa</v>
-      </c>
-      <c r="B36" t="str">
-        <v>Olu Ajasa</v>
-      </c>
-      <c r="C36" t="str">
-        <v>o.ajasa@giambronelaw.com</v>
-      </c>
-      <c r="D36" t="str">
-        <v>4402071839482</v>
-      </c>
-      <c r="E36" t="str">
-        <v>Giambrone International Law Firm</v>
-      </c>
-      <c r="G36" t="str">
-        <v>England</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>.</v>
-      </c>
-    </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="str">
-        <v>https://almtlegal.com/partner-sandhya-susanna-bhaskar-.htm</v>
-      </c>
-      <c r="B52" t="str">
-        <v>Sandhya Susanna Bhaskar</v>
-      </c>
-      <c r="C52" t="str">
-        <v>sbhaskar@almtlegal.com</v>
-      </c>
-      <c r="D52" t="str">
-        <v>918040160000</v>
-      </c>
-      <c r="E52" t="str">
-        <v>ALMT Legal</v>
-      </c>
-      <c r="G52" t="str">
-        <v>India</v>
+        <v>https://www.morganlewis.com/bios/nickbolter</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Nick Bolter</v>
+      </c>
+      <c r="C41" t="str">
+        <v>nick.bolter@morganlewis.com</v>
+      </c>
+      <c r="D41" t="str">
+        <v>442032015518</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Morgan Lewis And Bockius LLP</v>
+      </c>
+      <c r="G41" t="str">
+        <v>England</v>
       </c>
     </row>
   </sheetData>

</xml_diff>